<commit_message>
Refactor BiLevel arguments for consistency.
</commit_message>
<xml_diff>
--- a/tests/utils/study_inputs/disciplines_spec_options.xlsx
+++ b/tests/utils/study_inputs/disciplines_spec_options.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicolas.roussouly\Code\GEMSEO\GEMS-bliss\tests\utils\study_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gilberto.ruiz-j\PycharmProjects\gemseo\tests\utils\study_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -91,9 +91,6 @@
     <t>Options values</t>
   </si>
   <si>
-    <t>main_mda_class</t>
-  </si>
-  <si>
     <t>MDAGaussSeidel</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
   </si>
   <si>
     <t>my_test_scenario</t>
+  </si>
+  <si>
+    <t>main_mda_name</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="19.453125" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,7 +462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -470,12 +470,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -493,14 +493,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.54296875" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -508,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -532,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -547,16 +547,16 @@
   <dimension ref="B1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>13</v>
       </c>
@@ -579,7 +579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -596,13 +596,13 @@
         <v>17</v>
       </c>
       <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -610,39 +610,39 @@
         <v>18</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="L5" t="s">
-        <v>26</v>
       </c>
       <c r="M5" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6">
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M7">
         <v>20</v>

</xml_diff>